<commit_message>
some fix and some feature
</commit_message>
<xml_diff>
--- a/docs/docs.adoc.xlsx
+++ b/docs/docs.adoc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A08CDF0-7303-4ED5-B843-4BB816971AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044CE814-25CF-4660-96EC-A51D9FA437F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="23040" windowHeight="10752" activeTab="1" xr2:uid="{CDC06394-9021-4409-928C-5F2E0D4D7664}"/>
+    <workbookView xWindow="672" yWindow="8400" windowWidth="9252" windowHeight="3360" activeTab="1" xr2:uid="{CDC06394-9021-4409-928C-5F2E0D4D7664}"/>
   </bookViews>
   <sheets>
     <sheet name="errs" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="428">
   <si>
     <t>FLG</t>
   </si>
@@ -1082,21 +1082,6 @@
   </si>
   <si>
     <t>クリックして、base のモジュールと vbe のモジュールを比較できます。</t>
-  </si>
-  <si>
-    <t>最初に、右クリックして vbe と src を比較します。</t>
-  </si>
-  <si>
-    <t>src のモジュールを編集します。</t>
-  </si>
-  <si>
-    <t>右クリックして競合を解決します。</t>
-  </si>
-  <si>
-    <t>resolve コマンドは、vbe を base にコピーすることです。</t>
-  </si>
-  <si>
-    <t>解決コマンドは非常に混乱しています。ごめん。</t>
   </si>
   <si>
     <t>エディターのコンテキスト メニュー</t>
@@ -1356,6 +1341,76 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>confilicting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>When vbecm detects some confiliction between the source and the vbe,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>this tree is activate.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click this item, and show a diff tab between the source and the vbe.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The resolve command is removed on the latest version.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>解決コマンドは新しいバージョンでは、削除しました。</t>
+    <rPh sb="7" eb="8">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>サクジョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>競合</t>
+    <rPh sb="0" eb="2">
+      <t>キョウゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vbcmeは、VBEとSrcで競合を検知した場合は、confliction  treeが有効になります。</t>
+    <rPh sb="15" eb="17">
+      <t>キョウゴウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ケンチ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ユウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You edit the source and commit.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>競合個所を修正してから、コミットしてください。</t>
+    <rPh sb="0" eb="2">
+      <t>キョウゴウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カショ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1797,10 +1852,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC80C0-1AC7-484C-9D3D-1B9AD42320BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E238"/>
+  <dimension ref="A1:E248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="I221" sqref="I221"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1829,7 +1884,7 @@
         <v>286</v>
       </c>
       <c r="E2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -1924,21 +1979,21 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C23" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -2040,10 +2095,10 @@
       </c>
       <c r="B38"/>
       <c r="C38" s="7" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
@@ -2052,10 +2107,10 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B40"/>
       <c r="C40" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -2063,50 +2118,50 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B42"/>
       <c r="C42" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B43"/>
       <c r="C43" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B44"/>
       <c r="C44" s="3" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B45"/>
       <c r="C45" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -2894,37 +2949,28 @@
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B140"/>
       <c r="C140" s="2" t="s">
-        <v>38</v>
+        <v>422</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>349</v>
+        <v>423</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B141"/>
-      <c r="C141" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>350</v>
-      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B142"/>
-      <c r="C142" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>351</v>
-      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A143" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B143"/>
-      <c r="C143" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>352</v>
+      <c r="C143" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.45">
@@ -2933,235 +2979,214 @@
     <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B145"/>
       <c r="C145" s="2" t="s">
-        <v>41</v>
+        <v>419</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>353</v>
+        <v>425</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B146"/>
+      <c r="C146" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B147"/>
+      <c r="C147" s="2" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A148" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B148"/>
-      <c r="C148" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E148" s="7" t="s">
-        <v>354</v>
+      <c r="C148" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B149"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A150" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B150"/>
-      <c r="C150" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E150" s="3" t="s">
-        <v>355</v>
-      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A151" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B151"/>
-      <c r="C151" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A152" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B152"/>
-      <c r="C152" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E152" s="3" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A153" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B153"/>
-      <c r="C153" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A154" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B154"/>
-      <c r="C154" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>359</v>
-      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A155" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B155"/>
-      <c r="C155" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>360</v>
-      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A156" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B156"/>
-      <c r="C156" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>361</v>
-      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A157" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B157"/>
-      <c r="C157" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>362</v>
-      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A158" s="1" t="s">
-        <v>202</v>
+      <c r="A158" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="B158"/>
-      <c r="C158" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>363</v>
+      <c r="C158" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A159" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B159"/>
-      <c r="C159" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>364</v>
-      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A160" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B160"/>
       <c r="C160" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A161" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B161"/>
+      <c r="C161" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A162" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B162"/>
+      <c r="C162" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A163" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B163"/>
+      <c r="C163" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A164" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B164"/>
+      <c r="C164" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A165" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B165"/>
+      <c r="C165" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A166" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B166"/>
+      <c r="C166" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A167" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B167"/>
+      <c r="C167" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A168" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B168"/>
+      <c r="C168" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A169" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B169"/>
+      <c r="C169" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A170" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B170"/>
+      <c r="C170" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E160" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B161"/>
-      <c r="C161" s="2" t="s">
+      <c r="E170" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B171"/>
+      <c r="C171" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E161" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B162"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B163"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A164" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B164"/>
-      <c r="C164" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E164" s="7" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B165"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A166" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B166"/>
-      <c r="C166" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="E166" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B167"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B168"/>
-      <c r="C168" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B169"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B170"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A171" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B171"/>
-      <c r="C171" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="E171" s="7" t="s">
-        <v>370</v>
+      <c r="E171" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.45">
@@ -3169,74 +3194,62 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B173"/>
-      <c r="C173" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>371</v>
-      </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A174" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B174"/>
-      <c r="C174" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>372</v>
+      <c r="C174" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E174" s="7" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B175"/>
-      <c r="C175" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>373</v>
-      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A176" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B176"/>
+      <c r="C176" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E176" s="7" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A177" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="B177"/>
-      <c r="C177" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="E177" s="7" t="s">
-        <v>374</v>
-      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B178"/>
+      <c r="C178" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B179"/>
-      <c r="C179" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>375</v>
-      </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B180"/>
-      <c r="C180" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E180" s="2" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A181" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B181"/>
-      <c r="C181" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>377</v>
+      <c r="C181" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.45">
@@ -3244,73 +3257,77 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B183"/>
+      <c r="C183" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A184" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B184"/>
-      <c r="C184" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E184" s="7" t="s">
-        <v>378</v>
+      <c r="C184" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B185"/>
+      <c r="C185" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B186"/>
-      <c r="C186" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A187" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B187"/>
+      <c r="C187" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E187" s="7" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A188" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="B188"/>
-      <c r="C188" s="2"/>
-      <c r="E188" s="2"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B189"/>
-      <c r="C189" t="s">
-        <v>45</v>
-      </c>
-      <c r="E189" t="s">
-        <v>45</v>
+      <c r="C189" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B190"/>
-      <c r="C190" t="s">
-        <v>46</v>
-      </c>
-      <c r="E190" t="s">
-        <v>379</v>
+      <c r="C190" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B191"/>
-      <c r="C191" t="s">
-        <v>47</v>
-      </c>
-      <c r="E191" t="s">
-        <v>380</v>
+      <c r="C191" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A192" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="B192"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.45">
@@ -3322,154 +3339,153 @@
       </c>
       <c r="B194"/>
       <c r="C194" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E194" s="7" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B195"/>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A196" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B196"/>
-      <c r="C196" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>382</v>
+      <c r="C196" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A197" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B197"/>
-      <c r="C197" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E197" s="3" t="s">
-        <v>383</v>
-      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="B198"/>
-      <c r="C198" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E198" s="3" t="s">
-        <v>384</v>
-      </c>
+      <c r="C198" s="2"/>
+      <c r="E198" s="2"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B199"/>
-      <c r="C199" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>385</v>
+      <c r="C199" t="s">
+        <v>45</v>
+      </c>
+      <c r="E199" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A200" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B200"/>
-      <c r="C200" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="E200" s="3" t="s">
-        <v>386</v>
+      <c r="C200" t="s">
+        <v>46</v>
+      </c>
+      <c r="E200" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A201" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B201"/>
-      <c r="C201" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="E201" s="3" t="s">
-        <v>387</v>
+      <c r="C201" t="s">
+        <v>47</v>
+      </c>
+      <c r="E201" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A202" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B202"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A203" s="5" t="s">
+      <c r="B203"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A204" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B203"/>
-      <c r="C203" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E203" s="7" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B204"/>
+      <c r="C204" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E204" s="7" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B205"/>
-      <c r="C205" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A206" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B206"/>
+      <c r="C206" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A207" s="5" t="s">
-        <v>190</v>
+      <c r="A207" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B207"/>
-      <c r="C207" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E207" s="7" t="s">
-        <v>390</v>
+      <c r="C207" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A208" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B208"/>
+      <c r="C208" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B209"/>
       <c r="C209" s="2" t="s">
-        <v>61</v>
+        <v>261</v>
       </c>
       <c r="E209" s="2" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A210" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B210"/>
-      <c r="C210" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>392</v>
+      <c r="C210" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A211" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B211"/>
-      <c r="C211" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>393</v>
+      <c r="C211" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.45">
@@ -3477,14 +3493,14 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A213" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B213"/>
       <c r="C213" s="7" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E213" s="7" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.45">
@@ -3493,10 +3509,10 @@
     <row r="215" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B215"/>
       <c r="C215" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E215" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
@@ -3508,10 +3524,10 @@
       </c>
       <c r="B217"/>
       <c r="C217" s="7" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E217" s="7" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.45">
@@ -3520,136 +3536,208 @@
     <row r="219" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B219"/>
       <c r="C219" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B220"/>
+      <c r="C220" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A221" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B221"/>
-      <c r="C221" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="E221" s="7" t="s">
-        <v>398</v>
+      <c r="C221" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B222"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A223" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B223"/>
-      <c r="C223" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>399</v>
+      <c r="C223" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E223" s="7" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B224"/>
-      <c r="C224" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E224" s="2" t="s">
-        <v>400</v>
-      </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B225"/>
+      <c r="C225" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A226" s="5" t="s">
+      <c r="B226"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A227" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B226"/>
-      <c r="C226" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E226" s="7" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B227"/>
-      <c r="C227" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E227" s="2" t="s">
-        <v>402</v>
+      <c r="C227" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E227" s="7" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B228"/>
-      <c r="C228" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E228" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B229"/>
       <c r="C229" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B230"/>
-      <c r="C230" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E230" s="2" t="s">
-        <v>404</v>
-      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A231" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B231"/>
+      <c r="C231" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E231" s="7" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A232" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B232"/>
-      <c r="C232" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E232" s="7" t="s">
-        <v>405</v>
-      </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B233"/>
+      <c r="C233" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B234"/>
       <c r="C234" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B235"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A236" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B236"/>
+      <c r="C236" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E236" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B237"/>
+      <c r="C237" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B238"/>
+      <c r="C238" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B239"/>
+      <c r="C239" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B240"/>
+      <c r="C240" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B241"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A242" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B242"/>
+      <c r="C242" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E242" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B243"/>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B244"/>
+      <c r="C244" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E234" s="2" t="s">
+      <c r="E244" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C236" s="2"/>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C238" s="2"/>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C246" s="2"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C248" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:B24 A235:B1048576" xr:uid="{E5CD518D-F695-4AFF-BE3B-4E81514E7BF8}"/>
+    <dataValidation imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:B24 A245:B1048576" xr:uid="{E5CD518D-F695-4AFF-BE3B-4E81514E7BF8}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some fix, #11, #12, #13
</commit_message>
<xml_diff>
--- a/docs/docs.adoc.xlsx
+++ b/docs/docs.adoc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935B3D6-FEA2-42B3-859B-92217E0CF744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78A76BF-0C0F-437B-B370-9403E23281CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CDC06394-9021-4409-928C-5F2E0D4D7664}"/>
+    <workbookView xWindow="648" yWindow="120" windowWidth="17148" windowHeight="10524" activeTab="1" xr2:uid="{CDC06394-9021-4409-928C-5F2E0D4D7664}"/>
   </bookViews>
   <sheets>
     <sheet name="errs" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="444">
   <si>
     <t>FLG</t>
   </si>
@@ -1422,6 +1422,57 @@
       <t>ニホンゴ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vbecm: Auto Refresh Diff</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vbecm: Vbs Encode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vbecm: Diff Exclude</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Vbecm: Open Encoding Test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Set On, the diff tree view is refreshed automatically</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>When there are folders for not vba, the diff tree view detects them.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>you set the folder to exclude.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>For japanese. When the vscode opens files with non sjis encoding, it shows message.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If many mistake happen, please set off.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>オンに設定すると、差分ツリー ビューが自動的に更新されます</t>
+  </si>
+  <si>
+    <t>vba 以外のフォルダーがある場合は、差分ツリー ビューで検出されます。</t>
+  </si>
+  <si>
+    <t>除外するフォルダーを設定します。</t>
+  </si>
+  <si>
+    <t>日本人向け。 vscode が非 sjis エンコーディングのファイルを開くと、メッセージが表示されます。</t>
+  </si>
+  <si>
+    <t>ミスが多い場合は発進してください。</t>
   </si>
 </sst>
 </file>
@@ -1863,10 +1914,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC80C0-1AC7-484C-9D3D-1B9AD42320BA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1987,6 +2038,7 @@
       <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
@@ -2429,190 +2481,169 @@
       </c>
       <c r="B80"/>
       <c r="C80" s="3" t="s">
-        <v>201</v>
+        <v>430</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>306</v>
+        <v>430</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>202</v>
+        <v>408</v>
       </c>
       <c r="B81"/>
       <c r="C81" s="3" t="s">
-        <v>203</v>
+        <v>434</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>307</v>
+        <v>439</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B82"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="5" t="s">
-        <v>190</v>
+      <c r="A83" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B83"/>
-      <c r="C83" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>308</v>
+      <c r="C83" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B84"/>
+      <c r="C84" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B85"/>
       <c r="C85" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A86" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B86"/>
-      <c r="C86" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B87"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B88"/>
+      <c r="C88" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A89" s="5" t="s">
-        <v>184</v>
+      <c r="A89" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="B89"/>
-      <c r="C89" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>310</v>
+      <c r="C89" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B90"/>
+      <c r="C90" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B91"/>
-      <c r="C91" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B92"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A93" s="5" t="s">
-        <v>190</v>
+      <c r="A93" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B93"/>
-      <c r="C93" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>312</v>
+      <c r="C93" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
+        <v>408</v>
+      </c>
       <c r="B94"/>
+      <c r="C94" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A95" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B95"/>
-      <c r="C95" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>313</v>
+      <c r="C95" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A96" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B96"/>
-      <c r="C96" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A97" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B97"/>
-      <c r="C97" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>315</v>
-      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B98"/>
-      <c r="C98" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>316</v>
-      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A99" s="1" t="s">
-        <v>186</v>
+      <c r="A99" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="B99"/>
-      <c r="C99" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>317</v>
+      <c r="C99" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A100" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B100"/>
-      <c r="C100" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A101" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B101"/>
-      <c r="C101" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>319</v>
+      <c r="C101" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
@@ -2621,109 +2652,82 @@
       </c>
       <c r="B102"/>
       <c r="C102" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>320</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A103" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B103"/>
-      <c r="C103" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>321</v>
-      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A104" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B104"/>
-      <c r="C104" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>322</v>
-      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A105" s="1" t="s">
-        <v>186</v>
+      <c r="A105" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="B105"/>
-      <c r="C105" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>323</v>
+      <c r="C105" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A106" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B106"/>
-      <c r="C106" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A107" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B107"/>
-      <c r="C107" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>325</v>
+      <c r="C107" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B108"/>
-      <c r="C108" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>326</v>
-      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A109" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B109"/>
+      <c r="C109" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A110" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B110"/>
-      <c r="C110" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A111" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B111"/>
+      <c r="C111" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="B112"/>
       <c r="C112" s="3" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.45">
@@ -2732,22 +2736,19 @@
       </c>
       <c r="B113"/>
       <c r="C113" s="3" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A114" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B114"/>
-      <c r="C114" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>330</v>
+      <c r="C114" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
@@ -2756,10 +2757,10 @@
       </c>
       <c r="B115"/>
       <c r="C115" s="3" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
@@ -2768,34 +2769,34 @@
       </c>
       <c r="B116"/>
       <c r="C116" s="3" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="B117"/>
       <c r="C117" s="3" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B118"/>
       <c r="C118" s="3" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.45">
@@ -2804,157 +2805,220 @@
       </c>
       <c r="B119"/>
       <c r="C119" s="3" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="B120"/>
       <c r="C120" s="3" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B121"/>
       <c r="C121" s="3" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A122" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B122"/>
+      <c r="C122" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A123" s="5" t="s">
-        <v>190</v>
+      <c r="A123" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B123"/>
-      <c r="C123" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>338</v>
+      <c r="C123" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B124"/>
+      <c r="C124" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B125"/>
-      <c r="C125" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>339</v>
-      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A126" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B126"/>
+      <c r="C126" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A127" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="B127"/>
-      <c r="C127" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A128" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B128"/>
+      <c r="C128" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A129" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B129"/>
-      <c r="C129" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>341</v>
+      <c r="C129" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A130" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B130"/>
-      <c r="C130" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>342</v>
+      <c r="C130" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A131" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B131"/>
+      <c r="C131" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A132" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B132"/>
-      <c r="C132" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>343</v>
+      <c r="C132" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A133" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B133"/>
+      <c r="C133" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A134" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B134"/>
-      <c r="C134" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>344</v>
+      <c r="C134" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A135" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B135"/>
+      <c r="C135" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A136" s="5" t="s">
-        <v>234</v>
+      <c r="A136" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B136"/>
-      <c r="C136" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E136" s="7" t="s">
-        <v>345</v>
+      <c r="C136" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A137" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B137"/>
+      <c r="C137" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B138"/>
-      <c r="C138" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>346</v>
-      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A139" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B139"/>
-      <c r="C139" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>347</v>
+      <c r="C139" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.45">
@@ -2963,22 +3027,25 @@
     <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B141"/>
       <c r="C141" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B142"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A143" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B143"/>
-      <c r="C143" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>423</v>
+      <c r="C143" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.45">
@@ -2986,17 +3053,20 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B145"/>
+      <c r="C145" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A146" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="B146"/>
-      <c r="C146" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="E146" s="7" t="s">
-        <v>424</v>
+      <c r="C146" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.45">
@@ -3005,215 +3075,155 @@
     <row r="148" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B148"/>
       <c r="C148" s="2" t="s">
-        <v>419</v>
+        <v>34</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>425</v>
+        <v>343</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B149"/>
-      <c r="C149" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>427</v>
-      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B150"/>
       <c r="C150" s="2" t="s">
-        <v>421</v>
+        <v>236</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B151"/>
-      <c r="C151" s="2" t="s">
-        <v>426</v>
-      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A152" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B152"/>
+      <c r="C152" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B153"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B154"/>
+      <c r="C154" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B155"/>
+      <c r="C155" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B156"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B157"/>
+      <c r="C157" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B158"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B159"/>
+      <c r="C159" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B160"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A161" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B161"/>
-      <c r="C161" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E161" s="7" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A162" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B162"/>
+      <c r="C162" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A163" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B163"/>
-      <c r="C163" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>350</v>
-      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A164" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B164"/>
-      <c r="C164" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>351</v>
+      <c r="C164" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A165" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B165"/>
-      <c r="C165" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>352</v>
+      <c r="C165" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A166" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B166"/>
-      <c r="C166" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>353</v>
+      <c r="C166" s="2" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A167" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B167"/>
-      <c r="C167" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E167" s="3" t="s">
-        <v>354</v>
+      <c r="C167" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A168" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B168"/>
-      <c r="C168" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>355</v>
-      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A169" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B169"/>
-      <c r="C169" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A170" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B170"/>
-      <c r="C170" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>357</v>
-      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A171" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B171"/>
-      <c r="C171" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A172" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B172"/>
-      <c r="C172" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>359</v>
-      </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A173" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="B173"/>
-      <c r="C173" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>360</v>
-      </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B174"/>
-      <c r="C174" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>361</v>
-      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B175"/>
@@ -3227,100 +3237,154 @@
       </c>
       <c r="B177"/>
       <c r="C177" s="7" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="E177" s="7" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B178"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A179" s="5" t="s">
-        <v>234</v>
+      <c r="A179" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B179"/>
-      <c r="C179" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="E179" s="7" t="s">
-        <v>363</v>
+      <c r="C179" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A180" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B180"/>
+      <c r="C180" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A181" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B181"/>
-      <c r="C181" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>364</v>
+      <c r="C181" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A182" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B182"/>
+      <c r="C182" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A183" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B183"/>
+      <c r="C183" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A184" s="5" t="s">
-        <v>234</v>
+      <c r="A184" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B184"/>
-      <c r="C184" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="E184" s="7" t="s">
-        <v>365</v>
+      <c r="C184" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A185" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B185"/>
+      <c r="C185" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A186" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B186"/>
-      <c r="C186" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>366</v>
+      <c r="C186" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A187" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B187"/>
-      <c r="C187" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E187" s="2" t="s">
-        <v>367</v>
+      <c r="C187" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A188" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B188"/>
-      <c r="C188" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>368</v>
+      <c r="C188" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A189" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="B189"/>
+      <c r="C189" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A190" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="B190"/>
-      <c r="C190" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="E190" s="7" t="s">
-        <v>369</v>
+      <c r="C190" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.45">
@@ -3328,47 +3392,44 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B192"/>
-      <c r="C192" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E192" s="2" t="s">
-        <v>370</v>
-      </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A193" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B193"/>
-      <c r="C193" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E193" s="2" t="s">
-        <v>371</v>
+      <c r="C193" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B194"/>
-      <c r="C194" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>372</v>
-      </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A195" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B195"/>
+      <c r="C195" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B196"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A197" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B197"/>
-      <c r="C197" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E197" s="7" t="s">
-        <v>373</v>
+      <c r="C197" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.45">
@@ -3376,394 +3437,505 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B199"/>
-      <c r="C199" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A200" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B200"/>
+      <c r="C200" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E200" s="7" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A201" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="B201"/>
-      <c r="C201" s="2"/>
-      <c r="E201" s="2"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B202"/>
-      <c r="C202" t="s">
-        <v>45</v>
-      </c>
-      <c r="E202" t="s">
-        <v>45</v>
+      <c r="C202" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B203"/>
-      <c r="C203" t="s">
-        <v>46</v>
-      </c>
-      <c r="E203" t="s">
-        <v>374</v>
+      <c r="C203" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B204"/>
-      <c r="C204" t="s">
-        <v>47</v>
-      </c>
-      <c r="E204" t="s">
-        <v>375</v>
+      <c r="C204" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A205" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="B205"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A206" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="B206"/>
+      <c r="C206" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E206" s="7" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A207" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B207"/>
-      <c r="C207" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="E207" s="7" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B208"/>
+      <c r="C208" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A209" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B209"/>
-      <c r="C209" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E209" s="3" t="s">
-        <v>377</v>
+      <c r="C209" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A210" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B210"/>
-      <c r="C210" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E210" s="3" t="s">
-        <v>378</v>
+      <c r="C210" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A211" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B211"/>
-      <c r="C211" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>379</v>
-      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B212"/>
-      <c r="C212" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>380</v>
-      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A213" s="1" t="s">
-        <v>186</v>
+      <c r="A213" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="B213"/>
-      <c r="C213" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="E213" s="3" t="s">
-        <v>381</v>
+      <c r="C213" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E213" s="7" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A214" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="B214"/>
-      <c r="C214" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="E214" s="3" t="s">
-        <v>382</v>
-      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B215"/>
+      <c r="C215" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A216" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B216"/>
-      <c r="C216" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E216" s="7" t="s">
-        <v>383</v>
-      </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A217" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B217"/>
+      <c r="C217" s="2"/>
+      <c r="E217" s="2"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B218"/>
-      <c r="C218" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>384</v>
+      <c r="C218" t="s">
+        <v>45</v>
+      </c>
+      <c r="E218" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B219"/>
+      <c r="C219" t="s">
+        <v>46</v>
+      </c>
+      <c r="E219" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A220" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B220"/>
-      <c r="C220" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E220" s="7" t="s">
-        <v>385</v>
+      <c r="C220" t="s">
+        <v>47</v>
+      </c>
+      <c r="E220" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A221" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B221"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B222"/>
-      <c r="C222" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E222" s="2" t="s">
-        <v>386</v>
-      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A223" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="B223"/>
-      <c r="C223" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>387</v>
+      <c r="C223" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E223" s="7" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B224"/>
-      <c r="C224" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E224" s="2" t="s">
-        <v>388</v>
-      </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A225" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B225"/>
+      <c r="C225" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A226" s="5" t="s">
-        <v>190</v>
+      <c r="A226" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B226"/>
-      <c r="C226" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="E226" s="7" t="s">
-        <v>389</v>
+      <c r="C226" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A227" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B227"/>
+      <c r="C227" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B228"/>
       <c r="C228" s="2" t="s">
-        <v>50</v>
+        <v>261</v>
       </c>
       <c r="E228" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A229" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B229"/>
+      <c r="C229" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A230" s="5" t="s">
-        <v>190</v>
+      <c r="A230" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B230"/>
-      <c r="C230" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E230" s="7" t="s">
-        <v>391</v>
+      <c r="C230" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B231"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A232" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="B232"/>
-      <c r="C232" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E232" s="2" t="s">
-        <v>392</v>
+      <c r="C232" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E232" s="7" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B233"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A234" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B234"/>
-      <c r="C234" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="E234" s="7" t="s">
-        <v>393</v>
+      <c r="C234" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B235"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A236" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B236"/>
-      <c r="C236" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E236" s="2" t="s">
-        <v>394</v>
+      <c r="C236" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E236" s="7" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B237"/>
-      <c r="C237" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E237" s="2" t="s">
-        <v>395</v>
-      </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B238"/>
+      <c r="C238" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A239" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="B239"/>
-      <c r="C239" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E239" s="7" t="s">
-        <v>396</v>
+      <c r="C239" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B240"/>
       <c r="C240" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B241"/>
-      <c r="C241" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E241" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A242" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B242"/>
-      <c r="C242" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E242" s="2" t="s">
-        <v>398</v>
+      <c r="C242" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E242" s="7" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B243"/>
-      <c r="C243" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E243" s="2" t="s">
-        <v>399</v>
-      </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B244"/>
+      <c r="C244" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A245" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="B245"/>
-      <c r="C245" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E245" s="7" t="s">
-        <v>400</v>
-      </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A246" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="B246"/>
+      <c r="C246" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E246" s="7" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B247"/>
-      <c r="C247" s="2" t="s">
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B248"/>
+      <c r="C248" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B249"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A250" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B250"/>
+      <c r="C250" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E250" s="7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B251"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B252"/>
+      <c r="C252" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B253"/>
+      <c r="C253" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B254"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A255" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B255"/>
+      <c r="C255" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E255" s="7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B256"/>
+      <c r="C256" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B257"/>
+      <c r="C257" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B258"/>
+      <c r="C258" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B259"/>
+      <c r="C259" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B260"/>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A261" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B261"/>
+      <c r="C261" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E261" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B262"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B263"/>
+      <c r="C263" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E247" s="2" t="s">
+      <c r="E263" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C249" s="2"/>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C251" s="2"/>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C265" s="2"/>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C267" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">
-    <dataValidation imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:B24 A248:B1048576" xr:uid="{E5CD518D-F695-4AFF-BE3B-4E81514E7BF8}"/>
+    <dataValidation imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:B24 A264:B1048576" xr:uid="{E5CD518D-F695-4AFF-BE3B-4E81514E7BF8}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>